<commit_message>
edits LP master 23
</commit_message>
<xml_diff>
--- a/summer23/Lehrplanung-S23-Master.xlsx
+++ b/summer23/Lehrplanung-S23-Master.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/philipp/Nextcloud/LEHRPLANUNG_shared/S23/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pwunderlich/github/lehrplanung/summer23/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45C525EF-FFA6-6144-804F-77CD00ECD43A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D93B08D-4B6F-3A4A-8CCC-E15619F2159B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="500" windowWidth="21740" windowHeight="17500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14760" yWindow="2020" windowWidth="21740" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lehrangebot" sheetId="1" r:id="rId1"/>
@@ -460,10 +460,10 @@
     <t>Introduction to Social Sciences Methods: Statistics, text mining and WebScraping in R</t>
   </si>
   <si>
-    <t>Culture &amp; Values TBD</t>
-  </si>
-  <si>
     <t>Lehrplanung Sommersemester 2023</t>
+  </si>
+  <si>
+    <t>Emotional Strification</t>
   </si>
 </sst>
 </file>
@@ -635,10 +635,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -868,10 +868,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AR44"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" workbookViewId="0">
       <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
       <selection activeCell="E21" sqref="E21"/>
-      <selection pane="topRight" activeCell="I35" sqref="I35"/>
+      <selection pane="topRight" activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2325,8 +2325,8 @@
       <c r="AP39" s="9"/>
     </row>
     <row r="40" spans="1:42" ht="17" x14ac:dyDescent="0.2">
-      <c r="A40" s="26" t="s">
-        <v>50</v>
+      <c r="A40" s="27" t="s">
+        <v>37</v>
       </c>
       <c r="C40" s="21" t="s">
         <v>38</v>
@@ -2335,21 +2335,21 @@
       <c r="E40" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="G40" s="27" t="s">
-        <v>140</v>
-      </c>
-      <c r="H40" s="21" t="s">
-        <v>42</v>
+      <c r="G40" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="H40" s="27" t="s">
+        <v>51</v>
       </c>
       <c r="I40" s="1">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="J40" s="1">
         <v>2</v>
       </c>
       <c r="K40" s="1">
         <f t="shared" ref="K40" si="2">I40+J40</f>
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="AP40" s="9"/>
     </row>
@@ -2467,7 +2467,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -2482,8 +2482,8 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="28" t="s">
-        <v>141</v>
+      <c r="A2" s="26" t="s">
+        <v>140</v>
       </c>
       <c r="B2">
         <v>1</v>

</xml_diff>